<commit_message>
update: content lecture 17
</commit_message>
<xml_diff>
--- a/week-17/Week 17 Workshop Data.xlsx
+++ b/week-17/Week 17 Workshop Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FoS-POE-2\FoS-POE2\week-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\peter\ZDrive\00007717\Desktop\FoS-POE2\Week-17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BC6837-9821-4024-A56C-4A712F42B503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ex 2" sheetId="1" r:id="rId1"/>
@@ -18,11 +17,8 @@
     <sheet name="Ex 4" sheetId="4" r:id="rId3"/>
     <sheet name="Ex 5" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="66">
   <si>
     <t>Super</t>
   </si>
@@ -229,13 +225,19 @@
   </si>
   <si>
     <t>MSE</t>
+  </si>
+  <si>
+    <t>Sample (back-end)</t>
+  </si>
+  <si>
+    <t>Columns (front-end)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,7 +568,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,20 +631,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3" applyAlignment="1">
@@ -654,6 +644,19 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -961,25 +964,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -991,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9">
         <v>6</v>
@@ -1023,7 +1026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="12">
         <v>4</v>
@@ -1071,7 +1074,7 @@
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H6" s="28" t="s">
         <v>31</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>47</v>
       </c>
@@ -1108,15 +1111,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
       <c r="H8" s="28" t="s">
         <v>33</v>
       </c>
@@ -1134,15 +1137,15 @@
       </c>
       <c r="M8" s="33"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
       <c r="H9" s="28" t="s">
         <v>34</v>
       </c>
@@ -1159,28 +1162,28 @@
         <v>6.6666666666666625</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
       <c r="H11" s="29" t="s">
         <v>1</v>
       </c>
@@ -1189,15 +1192,15 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="H12" s="28" t="s">
         <v>31</v>
       </c>
@@ -1214,13 +1217,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
       <c r="H13" s="28" t="s">
         <v>32</v>
       </c>
@@ -1237,15 +1240,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="39" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
       <c r="H14" s="28" t="s">
         <v>33</v>
       </c>
@@ -1262,15 +1265,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
       <c r="H15" s="28" t="s">
         <v>34</v>
       </c>
@@ -1287,26 +1290,26 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1">
-      <c r="B17" s="34" t="s">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="16"/>
       <c r="H17" s="29" t="s">
         <v>30</v>
@@ -1315,7 +1318,7 @@
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>33</v>
       </c>
@@ -1431,13 +1434,13 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
       <c r="K22" s="28"/>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1520,7 +1523,7 @@
       <c r="H26" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="34">
         <v>16.333333333333314</v>
       </c>
       <c r="J26" s="28">
@@ -1539,7 +1542,7 @@
         <v>13.745022533304169</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>10.924766500838338</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>10.924766500838338</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1653,7 +1656,7 @@
       <c r="M29" s="28"/>
       <c r="N29" s="28"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>SUM(D24:D29)</f>
         <v>8.166615333413997</v>
@@ -1666,7 +1669,7 @@
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1">
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H31" s="30" t="s">
         <v>30</v>
       </c>
@@ -1681,7 +1684,7 @@
       <c r="M31" s="30"/>
       <c r="N31" s="30"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>8.0277588889000011</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>23.3610788889</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>13</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>17.361138888899998</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>10.0277988889</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>10.0277988889</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>16.333328666813998</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38">
         <f>SUM(D32:D37)</f>
         <v>8.1667133333999988</v>
@@ -1828,60 +1831,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15">
-      <c r="B2" s="40"/>
-      <c r="C2" s="41" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="36"/>
+      <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="37" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-    </row>
-    <row r="3" spans="2:15" ht="15" thickBot="1">
-      <c r="B3" s="40" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="38">
         <v>123</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="38">
         <v>138</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="38">
         <v>110</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="38">
         <v>151</v>
       </c>
       <c r="G3">
@@ -1889,20 +1892,20 @@
         <v>130.5</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
-      <c r="B4" s="40" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="38">
         <v>145</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="38">
         <v>165</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="38">
         <v>140</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="38">
         <v>167</v>
       </c>
       <c r="G4">
@@ -1925,20 +1928,20 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
-      <c r="B5" s="40" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="38">
         <v>156</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="38">
         <v>176</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="38">
         <v>185</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="38">
         <v>175</v>
       </c>
       <c r="G5">
@@ -1961,7 +1964,7 @@
         <v>317.66666666666669</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>188.91666666666666</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I7" s="28" t="s">
         <v>11</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>148.66666666666666</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -2026,7 +2029,7 @@
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>130.5</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>282.33333333333337</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>154.25</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>382.33333333333337</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>173</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="15" thickBot="1">
+    <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12">
         <f>SUM(D9:D11)</f>
         <v>907.29166667000004</v>
@@ -2149,12 +2152,12 @@
         <v>149.33333333333331</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="15" thickBot="1">
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>141.33330000000001</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>159.66669999999999</v>
       </c>
@@ -2201,7 +2204,7 @@
       <c r="I17" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="34">
         <v>3629.166666666667</v>
       </c>
       <c r="K17" s="28">
@@ -2220,7 +2223,7 @@
         <v>3.4633040700956501</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>145</v>
       </c>
@@ -2234,7 +2237,7 @@
       <c r="I18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="44">
+      <c r="J18" s="40">
         <v>1116.9166666666661</v>
       </c>
       <c r="K18" s="28">
@@ -2253,7 +2256,7 @@
         <v>3.2887615634582406</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="15">
         <v>164.33330000000001</v>
       </c>
@@ -2289,12 +2292,12 @@
       <c r="N19" s="28"/>
       <c r="O19" s="28"/>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>SUM(D16:D19)</f>
         <v>372.3059944499999</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="39">
         <f>D20*3</f>
         <v>1116.9179833499998</v>
       </c>
@@ -2314,7 +2317,7 @@
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
     </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1">
+    <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I21" s="30" t="s">
         <v>30</v>
       </c>
@@ -2338,21 +2341,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>12</v>
       </c>
@@ -2365,8 +2375,17 @@
       <c r="D1" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -2379,8 +2398,17 @@
       <c r="D2" s="8">
         <v>1234</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="G2" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>1234</v>
+      </c>
+      <c r="I2">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2393,8 +2421,30 @@
       <c r="D3" s="11">
         <v>1345</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="G3" s="41"/>
+      <c r="H3">
+        <v>1345</v>
+      </c>
+      <c r="I3">
+        <v>1745</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2407,8 +2457,22 @@
       <c r="D4" s="11">
         <v>1450</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="G4" s="41"/>
+      <c r="H4">
+        <v>1450</v>
+      </c>
+      <c r="I4">
+        <v>1690</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2421,8 +2485,32 @@
       <c r="D5" s="11">
         <v>1450</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="G5" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>1566</v>
+      </c>
+      <c r="I5">
+        <v>1101</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="28">
+        <v>3</v>
+      </c>
+      <c r="N5" s="28">
+        <v>3</v>
+      </c>
+      <c r="O5" s="28">
+        <v>3</v>
+      </c>
+      <c r="P5" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2435,8 +2523,30 @@
       <c r="D6" s="11">
         <v>1745</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="G6" s="41"/>
+      <c r="H6">
+        <v>1981</v>
+      </c>
+      <c r="I6">
+        <v>981</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="28">
+        <v>4029</v>
+      </c>
+      <c r="N6" s="28">
+        <v>5023</v>
+      </c>
+      <c r="O6" s="28">
+        <v>4493</v>
+      </c>
+      <c r="P6" s="28">
+        <v>13545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2449,8 +2559,30 @@
       <c r="D7" s="11">
         <v>1690</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="G7" s="41"/>
+      <c r="H7">
+        <v>1476</v>
+      </c>
+      <c r="I7">
+        <v>878</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="28">
+        <v>1343</v>
+      </c>
+      <c r="N7" s="28">
+        <v>1674.3333333333333</v>
+      </c>
+      <c r="O7" s="28">
+        <v>1497.6666666666667</v>
+      </c>
+      <c r="P7" s="28">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2463,8 +2595,32 @@
       <c r="D8" s="11">
         <v>1566</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="G8" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>1459</v>
+      </c>
+      <c r="I8">
+        <v>1893</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="28">
+        <v>11667</v>
+      </c>
+      <c r="N8" s="28">
+        <v>72558.333333333023</v>
+      </c>
+      <c r="O8" s="28">
+        <v>27042.333333333336</v>
+      </c>
+      <c r="P8" s="28">
+        <v>48431.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2477,8 +2633,20 @@
       <c r="D9" s="11">
         <v>1981</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="G9" s="41"/>
+      <c r="H9">
+        <v>1678</v>
+      </c>
+      <c r="I9">
+        <v>1652</v>
+      </c>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2491,8 +2659,22 @@
       <c r="D10" s="11">
         <v>1476</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="G10" s="41"/>
+      <c r="H10">
+        <v>1356</v>
+      </c>
+      <c r="I10">
+        <v>1462</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2505,8 +2687,23 @@
       <c r="D11" s="11">
         <v>1101</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="L11" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="28">
+        <v>3</v>
+      </c>
+      <c r="N11" s="28">
+        <v>3</v>
+      </c>
+      <c r="O11" s="28">
+        <v>3</v>
+      </c>
+      <c r="P11" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2519,8 +2716,33 @@
       <c r="D12" s="11">
         <v>981</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="G12" s="32"/>
+      <c r="H12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="28">
+        <v>4885</v>
+      </c>
+      <c r="N12" s="28">
+        <v>2960</v>
+      </c>
+      <c r="O12" s="28">
+        <v>5007</v>
+      </c>
+      <c r="P12" s="28">
+        <v>12852</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2533,8 +2755,35 @@
       <c r="D13" s="11">
         <v>878</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="G13" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="32">
+        <v>1234</v>
+      </c>
+      <c r="I13" s="32">
+        <v>1566</v>
+      </c>
+      <c r="J13" s="32">
+        <v>1459</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="28">
+        <v>1628.3333333333333</v>
+      </c>
+      <c r="N13" s="28">
+        <v>986.66666666666663</v>
+      </c>
+      <c r="O13" s="28">
+        <v>1669</v>
+      </c>
+      <c r="P13" s="28">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2547,8 +2796,33 @@
       <c r="D14" s="11">
         <v>1459</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="G14" s="45"/>
+      <c r="H14" s="32">
+        <v>1345</v>
+      </c>
+      <c r="I14" s="32">
+        <v>1981</v>
+      </c>
+      <c r="J14" s="32">
+        <v>1678</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="28">
+        <v>24608.333333333336</v>
+      </c>
+      <c r="N14" s="28">
+        <v>12456.333333333334</v>
+      </c>
+      <c r="O14" s="28">
+        <v>46657</v>
+      </c>
+      <c r="P14" s="28">
+        <v>130801.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2561,8 +2835,23 @@
       <c r="D15" s="11">
         <v>1678</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="G15" s="45"/>
+      <c r="H15" s="32">
+        <v>1450</v>
+      </c>
+      <c r="I15" s="32">
+        <v>1476</v>
+      </c>
+      <c r="J15" s="32">
+        <v>1356</v>
+      </c>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2575,8 +2864,26 @@
       <c r="D16" s="11">
         <v>1356</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="G16" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="32">
+        <v>1450</v>
+      </c>
+      <c r="I16" s="32">
+        <v>1101</v>
+      </c>
+      <c r="J16" s="32">
+        <v>1893</v>
+      </c>
+      <c r="L16" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2589,8 +2896,30 @@
       <c r="D17" s="11">
         <v>1893</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="G17" s="45"/>
+      <c r="H17" s="32">
+        <v>1745</v>
+      </c>
+      <c r="I17" s="32">
+        <v>981</v>
+      </c>
+      <c r="J17" s="32">
+        <v>1652</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="28">
+        <v>6</v>
+      </c>
+      <c r="N17" s="28">
+        <v>6</v>
+      </c>
+      <c r="O17" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2603,8 +2932,30 @@
       <c r="D18" s="11">
         <v>1652</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18" s="45"/>
+      <c r="H18" s="32">
+        <v>1690</v>
+      </c>
+      <c r="I18" s="32">
+        <v>878</v>
+      </c>
+      <c r="J18" s="32">
+        <v>1462</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="28">
+        <v>8914</v>
+      </c>
+      <c r="N18" s="28">
+        <v>7983</v>
+      </c>
+      <c r="O18" s="28">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2617,27 +2968,202 @@
       <c r="D19" s="14">
         <v>1462</v>
       </c>
+      <c r="L19" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="28">
+        <v>1485.6666666666667</v>
+      </c>
+      <c r="N19" s="28">
+        <v>1330.5</v>
+      </c>
+      <c r="O19" s="28">
+        <v>1583.3333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="28">
+        <v>38934.666666666788</v>
+      </c>
+      <c r="N20" s="28">
+        <v>175871.5</v>
+      </c>
+      <c r="O20" s="28">
+        <v>38286.266666666794</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L24" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="P24" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q24" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="R24" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L25" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="M25" s="28">
+        <v>26680.5</v>
+      </c>
+      <c r="N25" s="28">
+        <v>1</v>
+      </c>
+      <c r="O25" s="28">
+        <v>26680.5</v>
+      </c>
+      <c r="P25" s="28">
+        <v>0.82098337003049737</v>
+      </c>
+      <c r="Q25" s="28">
+        <v>0.38272585937055248</v>
+      </c>
+      <c r="R25" s="28">
+        <v>3.1765489310224262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M26" s="28">
+        <v>195080.33333333349</v>
+      </c>
+      <c r="N26" s="28">
+        <v>2</v>
+      </c>
+      <c r="O26" s="28">
+        <v>97540.166666666744</v>
+      </c>
+      <c r="P26" s="28">
+        <v>3.0014000765853881</v>
+      </c>
+      <c r="Q26" s="28">
+        <v>8.7709596585151206E-2</v>
+      </c>
+      <c r="R26" s="28">
+        <v>2.8067956057324186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L27" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" s="28">
+        <v>848802.99999999977</v>
+      </c>
+      <c r="N27" s="28">
+        <v>2</v>
+      </c>
+      <c r="O27" s="28">
+        <v>424401.49999999988</v>
+      </c>
+      <c r="P27" s="28">
+        <v>13.059222042915165</v>
+      </c>
+      <c r="Q27" s="28">
+        <v>9.7336669945901429E-4</v>
+      </c>
+      <c r="R27" s="28">
+        <v>2.8067956057324186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L28" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="M28" s="28">
+        <v>389978.66666666669</v>
+      </c>
+      <c r="N28" s="28">
+        <v>12</v>
+      </c>
+      <c r="O28" s="28">
+        <v>32498.222222222223</v>
+      </c>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L30" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="30">
+        <v>1460542.5</v>
+      </c>
+      <c r="N30" s="30">
+        <v>17</v>
+      </c>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="G8:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20" t="s">
@@ -2645,7 +3171,7 @@
       </c>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>22</v>
       </c>
@@ -2659,7 +3185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +3199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="9">
         <v>5</v>
@@ -2685,7 +3211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="9">
         <v>5</v>
@@ -2697,7 +3223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="9">
         <v>2</v>
@@ -2709,7 +3235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="12">
         <v>4</v>
@@ -2721,7 +3247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>26</v>
       </c>
@@ -2735,7 +3261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="9">
         <v>3</v>
@@ -2747,7 +3273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="9">
         <v>2</v>
@@ -2759,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="9">
         <v>1</v>
@@ -2771,7 +3297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="12">
         <v>2</v>

</xml_diff>